<commit_message>
Erste Lauffähige Version; muss noch "geschönt" werden
</commit_message>
<xml_diff>
--- a/fotoleuToolbox.xlsx
+++ b/fotoleuToolbox.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCA272C-6AF0-4B73-B36C-0F19A77CB468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C33930-41B2-4285-921D-435D25854740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="310">
   <si>
     <t>Empfangsschein</t>
   </si>
@@ -1073,6 +1073,15 @@
   </si>
   <si>
     <t>generateDocument: Document generated! 10 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz QR Code Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\doc4.docx at 04.01.2021 18:25:39</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 30 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\doc3.docx at 04.01.2021 19:49:45</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 04.01.2021 19:49:47</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 10 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz QR Code Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\doc4.docx at 04.01.2021 19:49:53</t>
   </si>
 </sst>
 </file>
@@ -18354,7 +18363,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C13067-15AF-4F78-98EF-8797820B2B84}">
-  <dimension ref="A2:H125"/>
+  <dimension ref="A2:H128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -18444,7 +18453,7 @@
     </row>
     <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -18456,7 +18465,7 @@
     </row>
     <row r="21" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>35</v>
@@ -18478,7 +18487,7 @@
     </row>
     <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -18490,7 +18499,7 @@
     </row>
     <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -18502,7 +18511,7 @@
     </row>
     <row r="24" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>35</v>
@@ -18524,7 +18533,7 @@
     </row>
     <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
@@ -18534,9 +18543,9 @@
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -18548,7 +18557,7 @@
     </row>
     <row r="27" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>35</v>
@@ -18568,9 +18577,9 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -18582,7 +18591,7 @@
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -18594,7 +18603,7 @@
     </row>
     <row r="30" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>35</v>
@@ -18616,7 +18625,7 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -18628,7 +18637,7 @@
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -18640,7 +18649,7 @@
     </row>
     <row r="33" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>35</v>
@@ -18662,7 +18671,7 @@
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -18674,7 +18683,7 @@
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -18684,43 +18693,43 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
     </row>
-    <row r="36" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
+        <v>293</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
     </row>
-    <row r="37" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
     </row>
-    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -18730,9 +18739,9 @@
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
     </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -18744,7 +18753,7 @@
     </row>
     <row r="40" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>35</v>
@@ -18764,9 +18773,9 @@
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
     </row>
-    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
@@ -18776,9 +18785,9 @@
       <c r="G41" s="21"/>
       <c r="H41" s="21"/>
     </row>
-    <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
@@ -18790,7 +18799,7 @@
     </row>
     <row r="43" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>35</v>
@@ -18810,9 +18819,9 @@
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
     </row>
-    <row r="44" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
@@ -18824,7 +18833,7 @@
     </row>
     <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
@@ -18836,7 +18845,7 @@
     </row>
     <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B46" s="22" t="s">
         <v>35</v>
@@ -18858,7 +18867,7 @@
     </row>
     <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -18870,7 +18879,7 @@
     </row>
     <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -18882,7 +18891,7 @@
     </row>
     <row r="49" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B49" s="22" t="s">
         <v>35</v>
@@ -18904,7 +18913,7 @@
     </row>
     <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
@@ -18916,7 +18925,7 @@
     </row>
     <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
@@ -18928,7 +18937,7 @@
     </row>
     <row r="52" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>35</v>
@@ -18950,7 +18959,7 @@
     </row>
     <row r="53" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
@@ -18962,7 +18971,7 @@
     </row>
     <row r="54" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
@@ -18974,7 +18983,7 @@
     </row>
     <row r="55" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B55" s="22" t="s">
         <v>35</v>
@@ -18996,7 +19005,7 @@
     </row>
     <row r="56" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
@@ -19008,7 +19017,7 @@
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
@@ -19020,7 +19029,7 @@
     </row>
     <row r="58" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B58" s="22" t="s">
         <v>35</v>
@@ -19042,7 +19051,7 @@
     </row>
     <row r="59" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
@@ -19052,9 +19061,9 @@
       <c r="G59" s="21"/>
       <c r="H59" s="21"/>
     </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
@@ -19064,43 +19073,43 @@
       <c r="G60" s="21"/>
       <c r="H60" s="21"/>
     </row>
-    <row r="61" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
+        <v>268</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G61" s="21"/>
       <c r="H61" s="21"/>
     </row>
-    <row r="62" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="B62" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D62" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E62" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F62" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
       <c r="G62" s="21"/>
       <c r="H62" s="21"/>
     </row>
-    <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
@@ -19110,9 +19119,9 @@
       <c r="G63" s="21"/>
       <c r="H63" s="21"/>
     </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B64" s="22"/>
       <c r="C64" s="22"/>
@@ -19124,7 +19133,7 @@
     </row>
     <row r="65" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B65" s="22" t="s">
         <v>35</v>
@@ -19144,9 +19153,9 @@
       <c r="G65" s="21"/>
       <c r="H65" s="21"/>
     </row>
-    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
@@ -19156,9 +19165,9 @@
       <c r="G66" s="21"/>
       <c r="H66" s="21"/>
     </row>
-    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
@@ -19168,43 +19177,43 @@
       <c r="G67" s="21"/>
       <c r="H67" s="21"/>
     </row>
-    <row r="68" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
+        <v>261</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G68" s="21"/>
       <c r="H68" s="21"/>
     </row>
-    <row r="69" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E69" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F69" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
       <c r="G69" s="21"/>
       <c r="H69" s="21"/>
     </row>
-    <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
@@ -19214,9 +19223,9 @@
       <c r="G70" s="21"/>
       <c r="H70" s="21"/>
     </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
@@ -19226,43 +19235,43 @@
       <c r="G71" s="21"/>
       <c r="H71" s="21"/>
     </row>
-    <row r="72" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
+        <v>257</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G72" s="21"/>
       <c r="H72" s="21"/>
     </row>
-    <row r="73" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F73" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
       <c r="G73" s="21"/>
       <c r="H73" s="21"/>
     </row>
-    <row r="74" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
@@ -19274,7 +19283,7 @@
     </row>
     <row r="75" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
@@ -19286,7 +19295,7 @@
     </row>
     <row r="76" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B76" s="22" t="s">
         <v>35</v>
@@ -19306,9 +19315,9 @@
       <c r="G76" s="21"/>
       <c r="H76" s="21"/>
     </row>
-    <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
@@ -19318,9 +19327,9 @@
       <c r="G77" s="21"/>
       <c r="H77" s="21"/>
     </row>
-    <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
@@ -19332,7 +19341,7 @@
     </row>
     <row r="79" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B79" s="22" t="s">
         <v>35</v>
@@ -19354,7 +19363,7 @@
     </row>
     <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
@@ -19366,7 +19375,7 @@
     </row>
     <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
@@ -19378,7 +19387,7 @@
     </row>
     <row r="82" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B82" s="22" t="s">
         <v>35</v>
@@ -19400,7 +19409,7 @@
     </row>
     <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
@@ -19410,31 +19419,21 @@
       <c r="G83" s="21"/>
       <c r="H83" s="21"/>
     </row>
-    <row r="84" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B84" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C84" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D84" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E84" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F84" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
       <c r="G84" s="21"/>
       <c r="H84" s="21"/>
     </row>
     <row r="85" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B85" s="22" t="s">
         <v>35</v>
@@ -19454,31 +19453,21 @@
       <c r="G85" s="21"/>
       <c r="H85" s="21"/>
     </row>
-    <row r="86" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="B86" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C86" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D86" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E86" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F86" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
       <c r="G86" s="21"/>
       <c r="H86" s="21"/>
     </row>
     <row r="87" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B87" s="22" t="s">
         <v>35</v>
@@ -19498,21 +19487,31 @@
       <c r="G87" s="21"/>
       <c r="H87" s="21"/>
     </row>
-    <row r="88" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="22"/>
+        <v>235</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F88" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G88" s="21"/>
       <c r="H88" s="21"/>
     </row>
     <row r="89" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B89" s="22" t="s">
         <v>35</v>
@@ -19532,21 +19531,31 @@
       <c r="G89" s="21"/>
       <c r="H89" s="21"/>
     </row>
-    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="B90" s="22"/>
-      <c r="C90" s="22"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="22"/>
+        <v>233</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D90" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E90" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F90" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G90" s="21"/>
       <c r="H90" s="21"/>
     </row>
     <row r="91" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B91" s="22"/>
       <c r="C91" s="22"/>
@@ -19556,21 +19565,31 @@
       <c r="G91" s="21"/>
       <c r="H91" s="21"/>
     </row>
-    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="B92" s="22"/>
-      <c r="C92" s="22"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="22"/>
+        <v>231</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F92" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G92" s="21"/>
       <c r="H92" s="21"/>
     </row>
     <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="20" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B93" s="22"/>
       <c r="C93" s="22"/>
@@ -19582,7 +19601,7 @@
     </row>
     <row r="94" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="20" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B94" s="22"/>
       <c r="C94" s="22"/>
@@ -19592,9 +19611,9 @@
       <c r="G94" s="21"/>
       <c r="H94" s="21"/>
     </row>
-    <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="20" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B95" s="22"/>
       <c r="C95" s="22"/>
@@ -19604,9 +19623,9 @@
       <c r="G95" s="21"/>
       <c r="H95" s="21"/>
     </row>
-    <row r="96" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="20" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B96" s="22"/>
       <c r="C96" s="22"/>
@@ -19616,75 +19635,45 @@
       <c r="G96" s="21"/>
       <c r="H96" s="21"/>
     </row>
-    <row r="97" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B97" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C97" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D97" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E97" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F97" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="B97" s="22"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
       <c r="G97" s="21"/>
       <c r="H97" s="21"/>
     </row>
-    <row r="98" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B98" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C98" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D98" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E98" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F98" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B98" s="22"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="22"/>
+      <c r="F98" s="22"/>
       <c r="G98" s="21"/>
       <c r="H98" s="21"/>
     </row>
-    <row r="99" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B99" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C99" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D99" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E99" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F99" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B99" s="22"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
       <c r="G99" s="21"/>
       <c r="H99" s="21"/>
     </row>
     <row r="100" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="20" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B100" s="22" t="s">
         <v>35</v>
@@ -19706,7 +19695,7 @@
     </row>
     <row r="101" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B101" s="22" t="s">
         <v>35</v>
@@ -19728,7 +19717,7 @@
     </row>
     <row r="102" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B102" s="22" t="s">
         <v>35</v>
@@ -19750,7 +19739,7 @@
     </row>
     <row r="103" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B103" s="22" t="s">
         <v>35</v>
@@ -19772,7 +19761,7 @@
     </row>
     <row r="104" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B104" s="22" t="s">
         <v>35</v>
@@ -19794,7 +19783,7 @@
     </row>
     <row r="105" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B105" s="22" t="s">
         <v>35</v>
@@ -19816,7 +19805,7 @@
     </row>
     <row r="106" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B106" s="22" t="s">
         <v>35</v>
@@ -19838,7 +19827,7 @@
     </row>
     <row r="107" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B107" s="22" t="s">
         <v>35</v>
@@ -19860,7 +19849,7 @@
     </row>
     <row r="108" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B108" s="22" t="s">
         <v>35</v>
@@ -19882,7 +19871,7 @@
     </row>
     <row r="109" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B109" s="22" t="s">
         <v>35</v>
@@ -19904,7 +19893,7 @@
     </row>
     <row r="110" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B110" s="22" t="s">
         <v>35</v>
@@ -19926,7 +19915,7 @@
     </row>
     <row r="111" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B111" s="22" t="s">
         <v>35</v>
@@ -19948,7 +19937,7 @@
     </row>
     <row r="112" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="20" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B112" s="22" t="s">
         <v>35</v>
@@ -19960,7 +19949,7 @@
         <v>49</v>
       </c>
       <c r="E112" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F112" s="22" t="s">
         <v>45</v>
@@ -19970,7 +19959,7 @@
     </row>
     <row r="113" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B113" s="22" t="s">
         <v>35</v>
@@ -19982,7 +19971,7 @@
         <v>49</v>
       </c>
       <c r="E113" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F113" s="22" t="s">
         <v>45</v>
@@ -19992,7 +19981,7 @@
     </row>
     <row r="114" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B114" s="22" t="s">
         <v>35</v>
@@ -20004,7 +19993,7 @@
         <v>49</v>
       </c>
       <c r="E114" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F114" s="22" t="s">
         <v>45</v>
@@ -20014,7 +20003,7 @@
     </row>
     <row r="115" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B115" s="22" t="s">
         <v>35</v>
@@ -20022,13 +20011,13 @@
       <c r="C115" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="21" t="s">
+      <c r="D115" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E115" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F115" s="21" t="s">
+      <c r="E115" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F115" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G115" s="21"/>
@@ -20036,7 +20025,7 @@
     </row>
     <row r="116" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B116" s="22" t="s">
         <v>35</v>
@@ -20044,13 +20033,13 @@
       <c r="C116" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D116" s="21" t="s">
+      <c r="D116" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E116" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F116" s="21" t="s">
+      <c r="E116" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F116" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G116" s="21"/>
@@ -20058,7 +20047,7 @@
     </row>
     <row r="117" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B117" s="22" t="s">
         <v>35</v>
@@ -20066,13 +20055,13 @@
       <c r="C117" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D117" s="21" t="s">
+      <c r="D117" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E117" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F117" s="21" t="s">
+      <c r="E117" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F117" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G117" s="21"/>
@@ -20080,7 +20069,7 @@
     </row>
     <row r="118" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B118" s="22" t="s">
         <v>35</v>
@@ -20102,7 +20091,7 @@
     </row>
     <row r="119" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B119" s="22" t="s">
         <v>35</v>
@@ -20124,7 +20113,7 @@
     </row>
     <row r="120" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A120" s="20" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B120" s="22" t="s">
         <v>35</v>
@@ -20146,7 +20135,7 @@
     </row>
     <row r="121" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A121" s="20" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B121" s="22" t="s">
         <v>35</v>
@@ -20155,7 +20144,7 @@
         <v>36</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E121" s="21" t="s">
         <v>44</v>
@@ -20168,7 +20157,7 @@
     </row>
     <row r="122" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B122" s="22" t="s">
         <v>35</v>
@@ -20176,27 +20165,43 @@
       <c r="C122" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D122" s="21"/>
-      <c r="E122" s="21"/>
-      <c r="F122" s="21"/>
+      <c r="D122" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E122" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F122" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G122" s="21"/>
       <c r="H122" s="21"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A123" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B123" s="21"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="21"/>
-      <c r="E123" s="21"/>
-      <c r="F123" s="21"/>
+        <v>48</v>
+      </c>
+      <c r="B123" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C123" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D123" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E123" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F123" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G123" s="21"/>
       <c r="H123" s="21"/>
     </row>
     <row r="124" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A124" s="20" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B124" s="22" t="s">
         <v>35</v>
@@ -20204,14 +20209,64 @@
       <c r="C124" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D124" s="21"/>
-      <c r="E124" s="21"/>
-      <c r="F124" s="21"/>
+      <c r="D124" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E124" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F124" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G124" s="21"/>
       <c r="H124" s="21"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="19" t="s">
+    <row r="125" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A125" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B125" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C125" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D125" s="21"/>
+      <c r="E125" s="21"/>
+      <c r="F125" s="21"/>
+      <c r="G125" s="21"/>
+      <c r="H125" s="21"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B126" s="21"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="21"/>
+      <c r="E126" s="21"/>
+      <c r="F126" s="21"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="21"/>
+    </row>
+    <row r="127" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A127" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B127" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D127" s="21"/>
+      <c r="E127" s="21"/>
+      <c r="F127" s="21"/>
+      <c r="G127" s="21"/>
+      <c r="H127" s="21"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="19" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avoid message box at word exit, after a combined document has been created.
</commit_message>
<xml_diff>
--- a/fotoleuToolbox.xlsx
+++ b/fotoleuToolbox.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C33930-41B2-4285-921D-435D25854740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34231BBD-7C79-432D-9E54-03EE706AF714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SwissQRCode (old)" sheetId="3" state="hidden" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="332">
   <si>
     <t>Empfangsschein</t>
   </si>
@@ -1082,6 +1082,72 @@
   </si>
   <si>
     <t>generateDocument: Document generated! 10 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz QR Code Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\doc4.docx at 04.01.2021 19:49:53</t>
+  </si>
+  <si>
+    <t>Muster</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Erliweg 99a</t>
+  </si>
+  <si>
+    <t>Steinhausen</t>
+  </si>
+  <si>
+    <t>fritz.peter@mymail.com</t>
+  </si>
+  <si>
+    <t>+41 79 999 888 77</t>
+  </si>
+  <si>
+    <t>KF0999</t>
+  </si>
+  <si>
+    <t>Erliweg 999a</t>
+  </si>
+  <si>
+    <t>fritz.pter@mymail.com</t>
+  </si>
+  <si>
+    <t>230.00</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 30 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\1stDoc_AF1571_e8b05e9c-b666-408e-92bb-d56b72753ef0.docx at 05.01.2021 12:02:10</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 05.01.2021 12:02:11</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 10 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz QR Code Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\2ndDoc_AF1571_e8b05e9c-b666-408e-92bb-d56b72753ef0.docx at 05.01.2021 12:02:17</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 30 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\1stDoc_AF1571_a0f85db4-93e9-4a7f-b16a-8ae8abb5c2f9.docx at 05.01.2021 12:04:42</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 05.01.2021 12:04:43</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 10 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz QR Code Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\2ndDoc_AF1571_a0f85db4-93e9-4a7f-b16a-8ae8abb5c2f9.docx at 05.01.2021 12:04:49</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 30 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\1stDoc_AF1571_c5f31efd-48f4-4f48-b552-4fbf0f481045.docx at 05.01.2021 12:06:07</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 05.01.2021 12:06:08</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 10 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz QR Code Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\2ndDoc_AF1571_c5f31efd-48f4-4f48-b552-4fbf0f481045.docx at 05.01.2021 12:06:15</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 30 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\1stDoc_AF1571_faa69c1c-7cba-49e3-a353-ee0540f884c6.docx at 05.01.2021 12:15:31</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 05.01.2021 12:15:33</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 10 bookmarks replaced. Template=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz QR Code Test Vorlage - Automatisiert.docx, Filepath=C:\Users\imfeldc\AppData\Local\Temp\2ndDoc_AF1571_faa69c1c-7cba-49e3-a353-ee0540f884c6.docx at 05.01.2021 12:15:39</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1396,7 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1419,13 +1485,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -2708,34 +2775,9 @@
             <v>Bösch 63</v>
           </cell>
         </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>6331 Hünenberg</v>
-          </cell>
-        </row>
         <row r="8">
           <cell r="A8" t="str">
             <v>AF1571 / KF0182 / ES=1353</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Moresi Aurelia</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Rigiweg 19a</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>5643  Sins</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>230</v>
           </cell>
         </row>
       </sheetData>
@@ -16816,8 +16858,8 @@
   </sheetPr>
   <dimension ref="B2:N97"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16924,33 +16966,26 @@
         <f t="array" ref="E12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Kunden ID (lang)],$E$13,1),"n/a")</f>
         <v>(KF0182) Moresi Aurelia</v>
       </c>
-      <c r="F12" s="33" t="str" cm="1">
-        <f t="array" ref="F12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Name],$E$13,1),"n/a")</f>
-        <v>Moresi</v>
-      </c>
-      <c r="G12" s="33" t="str" cm="1">
-        <f t="array" ref="G12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Vorname],$E$13,1),"n/a")</f>
-        <v>Aurelia</v>
-      </c>
-      <c r="H12" s="33" t="str" cm="1">
-        <f t="array" ref="H12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Adresse],$E$13,1),"n/a")</f>
-        <v>Rigiweg 19a</v>
-      </c>
-      <c r="I12" s="33" t="str" cm="1">
-        <f t="array" ref="I12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[PLZ],$E$13,1),"n/a")</f>
-        <v xml:space="preserve">5643 </v>
-      </c>
-      <c r="J12" s="33" t="str" cm="1">
-        <f t="array" ref="J12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Ort],$E$13,1),"n/a")</f>
-        <v>Sins</v>
-      </c>
-      <c r="K12" s="33" t="str" cm="1">
-        <f t="array" ref="K12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Mailadresse],$E$13,1),"n/a")</f>
-        <v>aurelia.moresi@gmx.ch</v>
-      </c>
-      <c r="L12" s="33" t="str" cm="1">
-        <f t="array" ref="L12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Telefonnummer],$E$13,1),"n/a")</f>
-        <v>+41 76 377 92 93</v>
+      <c r="F12" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="I12" s="33">
+        <v>6312</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="L12" s="50" t="s">
+        <v>315</v>
       </c>
       <c r="M12" s="33" t="str" cm="1">
         <f t="array" ref="M12">IF($D$12&lt;&gt;"",INDEX([1]!KundenTabelle[Kunden ID],$E$13,1),"n/a")</f>
@@ -17477,9 +17512,8 @@
       <c r="D68" t="s">
         <v>102</v>
       </c>
-      <c r="E68" t="str" cm="1">
-        <f t="array" ref="E68">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[Name],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[Name],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v>Moresi</v>
+      <c r="E68" t="s">
+        <v>310</v>
       </c>
       <c r="F68" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17491,9 +17525,8 @@
       <c r="D69" t="s">
         <v>103</v>
       </c>
-      <c r="E69" t="str" cm="1">
-        <f t="array" ref="E69">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[Vorname],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[Vorname],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v>Aurelia</v>
+      <c r="E69" t="s">
+        <v>311</v>
       </c>
       <c r="F69" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17504,9 +17537,8 @@
       <c r="D70" t="s">
         <v>104</v>
       </c>
-      <c r="E70" t="str" cm="1">
-        <f t="array" ref="E70">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[Adresse],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[Adresse],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v>Rigiweg 19a</v>
+      <c r="E70" t="s">
+        <v>312</v>
       </c>
       <c r="F70" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17517,9 +17549,8 @@
       <c r="D71" t="s">
         <v>105</v>
       </c>
-      <c r="E71" t="str" cm="1">
-        <f t="array" ref="E71">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[PLZ],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[PLZ],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v xml:space="preserve">5643 </v>
+      <c r="E71" s="45">
+        <v>6312</v>
       </c>
       <c r="F71" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17530,9 +17561,8 @@
       <c r="D72" t="s">
         <v>106</v>
       </c>
-      <c r="E72" t="str" cm="1">
-        <f t="array" ref="E72">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[Ort],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[Ort],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v>Sins</v>
+      <c r="E72" t="s">
+        <v>313</v>
       </c>
       <c r="F72" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17543,9 +17573,8 @@
       <c r="D73" t="s">
         <v>107</v>
       </c>
-      <c r="E73" t="str" cm="1">
-        <f t="array" ref="E73">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[Mailadresse],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[Mailadresse],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v>aurelia.moresi@gmx.ch</v>
+      <c r="E73" t="s">
+        <v>314</v>
       </c>
       <c r="F73" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17556,9 +17585,8 @@
       <c r="D74" t="s">
         <v>108</v>
       </c>
-      <c r="E74" t="str" cm="1">
-        <f t="array" ref="E74">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[Telefonnummer],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[Telefonnummer],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v>+41 76 377 92 93</v>
+      <c r="E74" s="27" t="s">
+        <v>315</v>
       </c>
       <c r="F74" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17569,9 +17597,8 @@
       <c r="D75" t="s">
         <v>114</v>
       </c>
-      <c r="E75" t="str" cm="1">
-        <f t="array" ref="E75">IFERROR(IF($D$12&lt;&gt;"",IF(INDEX([1]!KundenTabelle[Kunden ID],$E$13,1)&lt;&gt;0,INDEX([1]!KundenTabelle[Kunden ID],$E$13,1),$H$67),"n/a"),"n/v")</f>
-        <v>KF0182</v>
+      <c r="E75" t="s">
+        <v>316</v>
       </c>
       <c r="F75" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17673,7 +17700,7 @@
       <c r="D83" t="s">
         <v>204</v>
       </c>
-      <c r="E83" s="49" t="s">
+      <c r="E83" s="48" t="s">
         <v>225</v>
       </c>
       <c r="F83" s="46" t="str">
@@ -17762,8 +17789,8 @@
         <v>213</v>
       </c>
       <c r="E89" t="str">
-        <f>[1]SwissQRCode!A5</f>
-        <v>6331 Hünenberg</v>
+        <f>CONCATENATE(E71," ",E72)</f>
+        <v>6312 Steinhausen</v>
       </c>
       <c r="F89" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17775,8 +17802,8 @@
         <v>214</v>
       </c>
       <c r="E90" t="str">
-        <f>[1]SwissQRCode!A12</f>
-        <v>Moresi Aurelia</v>
+        <f>CONCATENATE(E68," ",E69)</f>
+        <v>Muster Peter</v>
       </c>
       <c r="F90" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17788,8 +17815,8 @@
         <v>215</v>
       </c>
       <c r="E91" t="str">
-        <f>[1]SwissQRCode!A13</f>
-        <v>Rigiweg 19a</v>
+        <f>E70</f>
+        <v>Erliweg 99a</v>
       </c>
       <c r="F91" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17801,8 +17828,8 @@
         <v>216</v>
       </c>
       <c r="E92" t="str">
-        <f>[1]SwissQRCode!A14</f>
-        <v>5643  Sins</v>
+        <f>CONCATENATE(E71," ",E72)</f>
+        <v>6312 Steinhausen</v>
       </c>
       <c r="F92" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17813,9 +17840,8 @@
       <c r="D93" t="s">
         <v>41</v>
       </c>
-      <c r="E93" s="48">
-        <f>[1]SwissQRCode!A17</f>
-        <v>230</v>
+      <c r="E93" s="51" t="s">
+        <v>319</v>
       </c>
       <c r="F93" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
@@ -17853,9 +17879,9 @@
       </c>
       <c r="E96" t="str">
         <f>CONCATENATE(E80,"_",E75,"_",E90,".docx")</f>
-        <v>AF1571_KF0182_Moresi Aurelia.docx</v>
-      </c>
-      <c r="F96" s="50" t="str">
+        <v>AF1571_KF0999_Muster Peter.docx</v>
+      </c>
+      <c r="F96" s="49" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
         <v>[--Filename--]</v>
       </c>
@@ -17867,7 +17893,7 @@
       <c r="E97" t="s">
         <v>223</v>
       </c>
-      <c r="F97" s="50" t="str">
+      <c r="F97" s="49" t="str">
         <f>CONCATENATE("[--",TabABBookmarks[[#This Row],[BookmarkName]],"--]")</f>
         <v>[--Filepath--]</v>
       </c>
@@ -18363,9 +18389,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C13067-15AF-4F78-98EF-8797820B2B84}">
-  <dimension ref="A2:H128"/>
+  <dimension ref="A2:H140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -18453,7 +18479,7 @@
     </row>
     <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -18465,7 +18491,7 @@
     </row>
     <row r="21" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>35</v>
@@ -18487,7 +18513,7 @@
     </row>
     <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -18499,7 +18525,7 @@
     </row>
     <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>306</v>
+        <v>328</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -18511,7 +18537,7 @@
     </row>
     <row r="24" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>35</v>
@@ -18533,7 +18559,7 @@
     </row>
     <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
@@ -18545,7 +18571,7 @@
     </row>
     <row r="26" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -18557,7 +18583,7 @@
     </row>
     <row r="27" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>35</v>
@@ -18579,7 +18605,7 @@
     </row>
     <row r="28" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -18589,9 +18615,9 @@
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -18603,7 +18629,7 @@
     </row>
     <row r="30" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>299</v>
+        <v>321</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>35</v>
@@ -18623,9 +18649,9 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -18635,9 +18661,9 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -18649,7 +18675,7 @@
     </row>
     <row r="33" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>35</v>
@@ -18669,9 +18695,9 @@
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -18681,9 +18707,9 @@
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
     </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -18695,7 +18721,7 @@
     </row>
     <row r="36" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>35</v>
@@ -18715,9 +18741,9 @@
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -18727,9 +18753,9 @@
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
     </row>
-    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -18739,43 +18765,43 @@
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
     </row>
-    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
+        <v>302</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
     </row>
-    <row r="40" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
     </row>
-    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
@@ -18785,43 +18811,43 @@
       <c r="G41" s="21"/>
       <c r="H41" s="21"/>
     </row>
-    <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
+        <v>299</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G42" s="21"/>
       <c r="H42" s="21"/>
     </row>
-    <row r="43" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
@@ -18831,43 +18857,43 @@
       <c r="G44" s="21"/>
       <c r="H44" s="21"/>
     </row>
-    <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
+        <v>296</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
     </row>
-    <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
     </row>
-    <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -18877,43 +18903,43 @@
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
+        <v>293</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
     </row>
-    <row r="49" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
       <c r="G49" s="21"/>
       <c r="H49" s="21"/>
     </row>
-    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
@@ -18925,7 +18951,7 @@
     </row>
     <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
@@ -18937,7 +18963,7 @@
     </row>
     <row r="52" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>35</v>
@@ -18959,7 +18985,7 @@
     </row>
     <row r="53" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
@@ -18969,9 +18995,9 @@
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
     </row>
-    <row r="54" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
@@ -18983,7 +19009,7 @@
     </row>
     <row r="55" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="B55" s="22" t="s">
         <v>35</v>
@@ -19003,9 +19029,9 @@
       <c r="G55" s="21"/>
       <c r="H55" s="21"/>
     </row>
-    <row r="56" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
@@ -19017,7 +19043,7 @@
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
@@ -19029,7 +19055,7 @@
     </row>
     <row r="58" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="B58" s="22" t="s">
         <v>35</v>
@@ -19051,7 +19077,7 @@
     </row>
     <row r="59" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
@@ -19063,7 +19089,7 @@
     </row>
     <row r="60" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
@@ -19075,7 +19101,7 @@
     </row>
     <row r="61" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>35</v>
@@ -19097,7 +19123,7 @@
     </row>
     <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
@@ -19107,9 +19133,9 @@
       <c r="G62" s="21"/>
       <c r="H62" s="21"/>
     </row>
-    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
@@ -19119,43 +19145,43 @@
       <c r="G63" s="21"/>
       <c r="H63" s="21"/>
     </row>
-    <row r="64" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="B64" s="22"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
+        <v>277</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G64" s="21"/>
       <c r="H64" s="21"/>
     </row>
-    <row r="65" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F65" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
       <c r="G65" s="21"/>
       <c r="H65" s="21"/>
     </row>
     <row r="66" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
@@ -19165,43 +19191,43 @@
       <c r="G66" s="21"/>
       <c r="H66" s="21"/>
     </row>
-    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
+        <v>274</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G67" s="21"/>
       <c r="H67" s="21"/>
     </row>
-    <row r="68" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F68" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
       <c r="G68" s="21"/>
       <c r="H68" s="21"/>
     </row>
-    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B69" s="22"/>
       <c r="C69" s="22"/>
@@ -19211,21 +19237,31 @@
       <c r="G69" s="21"/>
       <c r="H69" s="21"/>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="22"/>
+        <v>271</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G70" s="21"/>
       <c r="H70" s="21"/>
     </row>
     <row r="71" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
@@ -19235,43 +19271,43 @@
       <c r="G71" s="21"/>
       <c r="H71" s="21"/>
     </row>
-    <row r="72" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D72" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E72" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F72" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
       <c r="G72" s="21"/>
       <c r="H72" s="21"/>
     </row>
-    <row r="73" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
+        <v>268</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G73" s="21"/>
       <c r="H73" s="21"/>
     </row>
-    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
@@ -19281,9 +19317,9 @@
       <c r="G74" s="21"/>
       <c r="H74" s="21"/>
     </row>
-    <row r="75" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
@@ -19293,43 +19329,43 @@
       <c r="G75" s="21"/>
       <c r="H75" s="21"/>
     </row>
-    <row r="76" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F76" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
       <c r="G76" s="21"/>
       <c r="H76" s="21"/>
     </row>
-    <row r="77" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="B77" s="22"/>
-      <c r="C77" s="22"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="22"/>
+        <v>264</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G77" s="21"/>
       <c r="H77" s="21"/>
     </row>
     <row r="78" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
@@ -19339,43 +19375,43 @@
       <c r="G78" s="21"/>
       <c r="H78" s="21"/>
     </row>
-    <row r="79" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="B79" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D79" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E79" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F79" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
       <c r="G79" s="21"/>
       <c r="H79" s="21"/>
     </row>
-    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
+        <v>261</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F80" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G80" s="21"/>
       <c r="H80" s="21"/>
     </row>
     <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
@@ -19385,31 +19421,21 @@
       <c r="G81" s="21"/>
       <c r="H81" s="21"/>
     </row>
-    <row r="82" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="B82" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D82" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F82" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
       <c r="G82" s="21"/>
       <c r="H82" s="21"/>
     </row>
-    <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
@@ -19419,43 +19445,43 @@
       <c r="G83" s="21"/>
       <c r="H83" s="21"/>
     </row>
-    <row r="84" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="B84" s="22"/>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
+        <v>257</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D84" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E84" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F84" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G84" s="21"/>
       <c r="H84" s="21"/>
     </row>
-    <row r="85" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="B85" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C85" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D85" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E85" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F85" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
       <c r="G85" s="21"/>
       <c r="H85" s="21"/>
     </row>
-    <row r="86" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
@@ -19465,31 +19491,21 @@
       <c r="G86" s="21"/>
       <c r="H86" s="21"/>
     </row>
-    <row r="87" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B87" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D87" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E87" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F87" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
       <c r="G87" s="21"/>
       <c r="H87" s="21"/>
     </row>
     <row r="88" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="B88" s="22" t="s">
         <v>35</v>
@@ -19509,87 +19525,67 @@
       <c r="G88" s="21"/>
       <c r="H88" s="21"/>
     </row>
-    <row r="89" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="B89" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D89" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E89" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F89" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="22"/>
       <c r="G89" s="21"/>
       <c r="H89" s="21"/>
     </row>
-    <row r="90" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="B90" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C90" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D90" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E90" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F90" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="B90" s="22"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="22"/>
       <c r="G90" s="21"/>
       <c r="H90" s="21"/>
     </row>
-    <row r="91" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="B91" s="22"/>
-      <c r="C91" s="22"/>
-      <c r="D91" s="22"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="22"/>
+        <v>250</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D91" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E91" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F91" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G91" s="21"/>
       <c r="H91" s="21"/>
     </row>
-    <row r="92" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="B92" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C92" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D92" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E92" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F92" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
       <c r="G92" s="21"/>
       <c r="H92" s="21"/>
     </row>
     <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="20" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="B93" s="22"/>
       <c r="C93" s="22"/>
@@ -19599,21 +19595,31 @@
       <c r="G93" s="21"/>
       <c r="H93" s="21"/>
     </row>
-    <row r="94" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A94" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="B94" s="22"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="22"/>
+        <v>247</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D94" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F94" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G94" s="21"/>
       <c r="H94" s="21"/>
     </row>
     <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="20" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="B95" s="22"/>
       <c r="C95" s="22"/>
@@ -19625,7 +19631,7 @@
     </row>
     <row r="96" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="20" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="B96" s="22"/>
       <c r="C96" s="22"/>
@@ -19635,21 +19641,31 @@
       <c r="G96" s="21"/>
       <c r="H96" s="21"/>
     </row>
-    <row r="97" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A97" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="B97" s="22"/>
-      <c r="C97" s="22"/>
-      <c r="D97" s="22"/>
-      <c r="E97" s="22"/>
-      <c r="F97" s="22"/>
+        <v>244</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E97" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F97" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G97" s="21"/>
       <c r="H97" s="21"/>
     </row>
-    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="20" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="B98" s="22"/>
       <c r="C98" s="22"/>
@@ -19659,21 +19675,31 @@
       <c r="G98" s="21"/>
       <c r="H98" s="21"/>
     </row>
-    <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="B99" s="22"/>
-      <c r="C99" s="22"/>
-      <c r="D99" s="22"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="22"/>
+        <v>236</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F99" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G99" s="21"/>
       <c r="H99" s="21"/>
     </row>
     <row r="100" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="20" t="s">
-        <v>94</v>
+        <v>235</v>
       </c>
       <c r="B100" s="22" t="s">
         <v>35</v>
@@ -19695,7 +19721,7 @@
     </row>
     <row r="101" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="s">
-        <v>93</v>
+        <v>234</v>
       </c>
       <c r="B101" s="22" t="s">
         <v>35</v>
@@ -19717,7 +19743,7 @@
     </row>
     <row r="102" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="B102" s="22" t="s">
         <v>35</v>
@@ -19737,31 +19763,21 @@
       <c r="G102" s="21"/>
       <c r="H102" s="21"/>
     </row>
-    <row r="103" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B103" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C103" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D103" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E103" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F103" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="22"/>
       <c r="G103" s="21"/>
       <c r="H103" s="21"/>
     </row>
     <row r="104" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="s">
-        <v>90</v>
+        <v>231</v>
       </c>
       <c r="B104" s="22" t="s">
         <v>35</v>
@@ -19781,163 +19797,93 @@
       <c r="G104" s="21"/>
       <c r="H104" s="21"/>
     </row>
-    <row r="105" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B105" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C105" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D105" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E105" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F105" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="B105" s="22"/>
+      <c r="C105" s="22"/>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
       <c r="G105" s="21"/>
       <c r="H105" s="21"/>
     </row>
-    <row r="106" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B106" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C106" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D106" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E106" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F106" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B106" s="22"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="22"/>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
       <c r="G106" s="21"/>
       <c r="H106" s="21"/>
     </row>
-    <row r="107" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B107" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C107" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D107" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E107" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F107" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B107" s="22"/>
+      <c r="C107" s="22"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="22"/>
       <c r="G107" s="21"/>
       <c r="H107" s="21"/>
     </row>
-    <row r="108" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B108" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C108" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D108" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E108" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F108" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B108" s="22"/>
+      <c r="C108" s="22"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="22"/>
       <c r="G108" s="21"/>
       <c r="H108" s="21"/>
     </row>
-    <row r="109" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B109" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C109" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D109" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E109" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F109" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="B109" s="22"/>
+      <c r="C109" s="22"/>
+      <c r="D109" s="22"/>
+      <c r="E109" s="22"/>
+      <c r="F109" s="22"/>
       <c r="G109" s="21"/>
       <c r="H109" s="21"/>
     </row>
-    <row r="110" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B110" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C110" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D110" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E110" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F110" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B110" s="22"/>
+      <c r="C110" s="22"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="22"/>
+      <c r="F110" s="22"/>
       <c r="G110" s="21"/>
       <c r="H110" s="21"/>
     </row>
-    <row r="111" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B111" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C111" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D111" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E111" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F111" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B111" s="22"/>
+      <c r="C111" s="22"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
       <c r="G111" s="21"/>
       <c r="H111" s="21"/>
     </row>
     <row r="112" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="20" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B112" s="22" t="s">
         <v>35</v>
@@ -19959,7 +19905,7 @@
     </row>
     <row r="113" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B113" s="22" t="s">
         <v>35</v>
@@ -19981,7 +19927,7 @@
     </row>
     <row r="114" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="B114" s="22" t="s">
         <v>35</v>
@@ -20003,7 +19949,7 @@
     </row>
     <row r="115" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B115" s="22" t="s">
         <v>35</v>
@@ -20015,7 +19961,7 @@
         <v>49</v>
       </c>
       <c r="E115" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F115" s="22" t="s">
         <v>45</v>
@@ -20025,7 +19971,7 @@
     </row>
     <row r="116" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="B116" s="22" t="s">
         <v>35</v>
@@ -20037,7 +19983,7 @@
         <v>49</v>
       </c>
       <c r="E116" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F116" s="22" t="s">
         <v>45</v>
@@ -20047,7 +19993,7 @@
     </row>
     <row r="117" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="B117" s="22" t="s">
         <v>35</v>
@@ -20059,7 +20005,7 @@
         <v>49</v>
       </c>
       <c r="E117" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F117" s="22" t="s">
         <v>45</v>
@@ -20069,7 +20015,7 @@
     </row>
     <row r="118" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="B118" s="22" t="s">
         <v>35</v>
@@ -20077,13 +20023,13 @@
       <c r="C118" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D118" s="21" t="s">
+      <c r="D118" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E118" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F118" s="21" t="s">
+      <c r="E118" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F118" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G118" s="21"/>
@@ -20091,7 +20037,7 @@
     </row>
     <row r="119" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B119" s="22" t="s">
         <v>35</v>
@@ -20099,13 +20045,13 @@
       <c r="C119" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D119" s="21" t="s">
+      <c r="D119" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E119" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F119" s="21" t="s">
+      <c r="E119" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F119" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G119" s="21"/>
@@ -20113,7 +20059,7 @@
     </row>
     <row r="120" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A120" s="20" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="B120" s="22" t="s">
         <v>35</v>
@@ -20121,13 +20067,13 @@
       <c r="C120" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D120" s="21" t="s">
+      <c r="D120" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E120" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F120" s="21" t="s">
+      <c r="E120" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F120" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G120" s="21"/>
@@ -20135,7 +20081,7 @@
     </row>
     <row r="121" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A121" s="20" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B121" s="22" t="s">
         <v>35</v>
@@ -20143,13 +20089,13 @@
       <c r="C121" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D121" s="21" t="s">
+      <c r="D121" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E121" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F121" s="21" t="s">
+      <c r="E121" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F121" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G121" s="21"/>
@@ -20157,7 +20103,7 @@
     </row>
     <row r="122" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B122" s="22" t="s">
         <v>35</v>
@@ -20165,13 +20111,13 @@
       <c r="C122" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D122" s="21" t="s">
+      <c r="D122" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E122" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F122" s="21" t="s">
+      <c r="E122" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F122" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G122" s="21"/>
@@ -20179,7 +20125,7 @@
     </row>
     <row r="123" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A123" s="20" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B123" s="22" t="s">
         <v>35</v>
@@ -20187,13 +20133,13 @@
       <c r="C123" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D123" s="21" t="s">
+      <c r="D123" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E123" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F123" s="21" t="s">
+      <c r="E123" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F123" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G123" s="21"/>
@@ -20201,7 +20147,7 @@
     </row>
     <row r="124" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A124" s="20" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B124" s="22" t="s">
         <v>35</v>
@@ -20209,13 +20155,13 @@
       <c r="C124" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D124" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E124" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F124" s="21" t="s">
+      <c r="D124" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E124" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F124" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G124" s="21"/>
@@ -20223,7 +20169,7 @@
     </row>
     <row r="125" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A125" s="20" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B125" s="22" t="s">
         <v>35</v>
@@ -20231,27 +20177,43 @@
       <c r="C125" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D125" s="21"/>
-      <c r="E125" s="21"/>
-      <c r="F125" s="21"/>
+      <c r="D125" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E125" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F125" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G125" s="21"/>
       <c r="H125" s="21"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A126" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B126" s="21"/>
-      <c r="C126" s="21"/>
-      <c r="D126" s="21"/>
-      <c r="E126" s="21"/>
-      <c r="F126" s="21"/>
+        <v>70</v>
+      </c>
+      <c r="B126" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D126" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E126" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F126" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G126" s="21"/>
       <c r="H126" s="21"/>
     </row>
     <row r="127" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A127" s="20" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B127" s="22" t="s">
         <v>35</v>
@@ -20259,14 +20221,262 @@
       <c r="C127" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D127" s="21"/>
-      <c r="E127" s="21"/>
-      <c r="F127" s="21"/>
+      <c r="D127" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E127" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F127" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G127" s="21"/>
       <c r="H127" s="21"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="19" t="s">
+    <row r="128" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A128" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B128" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D128" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E128" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F128" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G128" s="21"/>
+      <c r="H128" s="21"/>
+    </row>
+    <row r="129" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A129" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B129" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C129" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D129" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E129" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F129" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G129" s="21"/>
+      <c r="H129" s="21"/>
+    </row>
+    <row r="130" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A130" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B130" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C130" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D130" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E130" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F130" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G130" s="21"/>
+      <c r="H130" s="21"/>
+    </row>
+    <row r="131" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A131" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B131" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C131" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D131" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E131" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F131" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G131" s="21"/>
+      <c r="H131" s="21"/>
+    </row>
+    <row r="132" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A132" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B132" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D132" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E132" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F132" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G132" s="21"/>
+      <c r="H132" s="21"/>
+    </row>
+    <row r="133" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A133" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B133" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E133" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F133" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G133" s="21"/>
+      <c r="H133" s="21"/>
+    </row>
+    <row r="134" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A134" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B134" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C134" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D134" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E134" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F134" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G134" s="21"/>
+      <c r="H134" s="21"/>
+    </row>
+    <row r="135" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A135" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B135" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C135" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D135" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E135" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F135" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G135" s="21"/>
+      <c r="H135" s="21"/>
+    </row>
+    <row r="136" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A136" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B136" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C136" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D136" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E136" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F136" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G136" s="21"/>
+      <c r="H136" s="21"/>
+    </row>
+    <row r="137" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A137" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B137" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C137" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D137" s="21"/>
+      <c r="E137" s="21"/>
+      <c r="F137" s="21"/>
+      <c r="G137" s="21"/>
+      <c r="H137" s="21"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B138" s="21"/>
+      <c r="C138" s="21"/>
+      <c r="D138" s="21"/>
+      <c r="E138" s="21"/>
+      <c r="F138" s="21"/>
+      <c r="G138" s="21"/>
+      <c r="H138" s="21"/>
+    </row>
+    <row r="139" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A139" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B139" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C139" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D139" s="21"/>
+      <c r="E139" s="21"/>
+      <c r="F139" s="21"/>
+      <c r="G139" s="21"/>
+      <c r="H139" s="21"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="19" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>